<commit_message>
extract most recent Gini-coefficients; delete data older than 2010
</commit_message>
<xml_diff>
--- a/Separate_Data/Gini_coefficient_various_years.xlsx
+++ b/Separate_Data/Gini_coefficient_various_years.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main Directory\Random Stuff\Countries_Data_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main_Directory\Random_Stuff\Countries_Data_Analysis\Separate_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F468F473-A791-41CE-B474-0F91752FCA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B0EB48-1759-4E6D-B78A-786F574125B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10598" yWindow="10702" windowWidth="20714" windowHeight="13156" xr2:uid="{64934366-BA66-4852-B5CA-11F3B9A2B437}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{64934366-BA66-4852-B5CA-11F3B9A2B437}"/>
   </bookViews>
   <sheets>
     <sheet name="economic-inequality-gini-index" sheetId="1" r:id="rId1"/>
+    <sheet name="most-recent-gini-since-2010" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4520" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="358">
   <si>
     <t>Entity</t>
   </si>
@@ -1101,7 +1102,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1583,7 +1584,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1629,9 +1630,15 @@
     <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.00000000"/>
+      <numFmt numFmtId="164" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1653,10 +1660,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35549655-227D-4499-9AFA-7371338876DE}" name="Tabelle2" displayName="Tabelle2" ref="A1:D2312" totalsRowShown="0">
   <autoFilter ref="A1:D2312" xr:uid="{35549655-227D-4499-9AFA-7371338876DE}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F66B3A32-AC6C-483E-AD07-4C043AD15D57}" name="Entity" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{F66B3A32-AC6C-483E-AD07-4C043AD15D57}" name="Entity" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{BACC2A4C-6838-4D37-89FC-8227393A7F7E}" name="Code"/>
     <tableColumn id="3" xr3:uid="{B458445A-012F-4853-9382-D9248633C18E}" name="Year"/>
-    <tableColumn id="4" xr3:uid="{C83C6566-144C-4803-9064-2C9E9B520BC5}" name="Gini coefficient (2021 prices) - Income or consumption consolidated" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{C83C6566-144C-4803-9064-2C9E9B520BC5}" name="Gini coefficient (2021 prices) - Income or consumption consolidated" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B6636B3-3D4A-48F7-B3B4-2FAFAA902C46}" name="Tabelle22" displayName="Tabelle22" ref="A1:D169" totalsRowShown="0">
+  <autoFilter ref="A1:D169" xr:uid="{7B6636B3-3D4A-48F7-B3B4-2FAFAA902C46}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D169">
+    <sortCondition descending="1" ref="D1:D169"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6715D57B-DD7A-4EFC-9074-75D85F7D57AA}" name="Entity" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1B313C84-FF2B-40F1-A63F-5791AAFF0A0F}" name="Code"/>
+    <tableColumn id="3" xr3:uid="{5DDC9EB7-5E68-46DB-B44B-B654D348312D}" name="Year"/>
+    <tableColumn id="4" xr3:uid="{4191979C-0328-48AE-941D-6D30DC093EDE}" name="Gini coefficient (2021 prices) - Income or consumption consolidated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1981,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16070F0C-BD73-4BBC-96DE-946F6A2A48C2}">
   <dimension ref="A1:D2312"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34050,4 +34073,2385 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1015EEBD-542C-4939-A935-715341BF2E6D}">
+  <dimension ref="A1:D169"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.63025719999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3">
+        <v>2012</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.60450804000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.59066609999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>2015</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.54907360000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6">
+        <v>2016</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.54579794000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>2023</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.53881924999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>2023</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.51639440000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C9">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.51484949999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>2018</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.51264286000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C11">
+        <v>2015</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.51225065999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C12">
+        <v>2019</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.50263760000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C13">
+        <v>2019</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.50256449999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14">
+        <v>2021</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.49384618000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>2011</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.48937692999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C16">
+        <v>2023</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.48875666000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17">
+        <v>2023</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.46826827999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18">
+        <v>2014</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.46156292999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19">
+        <v>2024</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.45829140000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20">
+        <v>2014</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.45332187000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <v>2023</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.45212682999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22">
+        <v>2017</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.44877613</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23">
+        <v>2020</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.44673239999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24">
+        <v>2023</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.44579553999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C25">
+        <v>2022</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.44467676</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26">
+        <v>2023</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.44382226000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C27">
+        <v>2016</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.44047811999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28">
+        <v>2018</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.4381641</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C29">
+        <v>2016</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.43709510000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30">
+        <v>2016</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.43508595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31">
+        <v>2022</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.43454006000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32">
+        <v>2022</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.43042782000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33">
+        <v>2021</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.43034457999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B34" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34">
+        <v>2019</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.42702177000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35">
+        <v>2012</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.42533894999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>2023</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.42390974999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37">
+        <v>2015</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.42381087000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38">
+        <v>2021</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.42176074000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>2023</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.42050114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B40" t="s">
+        <v>340</v>
+      </c>
+      <c r="C40">
+        <v>2023</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.41818877999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41">
+        <v>2017</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.41586014999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B42" t="s">
+        <v>342</v>
+      </c>
+      <c r="C42">
+        <v>2023</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.40867536999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B43" t="s">
+        <v>273</v>
+      </c>
+      <c r="C43">
+        <v>2017</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.40729480000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C44">
+        <v>2021</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.40668428000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B45" t="s">
+        <v>252</v>
+      </c>
+      <c r="C45">
+        <v>2023</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.40657840000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B46" t="s">
+        <v>314</v>
+      </c>
+      <c r="C46">
+        <v>2018</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.4049123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B47" t="s">
+        <v>209</v>
+      </c>
+      <c r="C47">
+        <v>2013</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.40052038000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>2018</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.39949583999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49">
+        <v>2021</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.39874472999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50">
+        <v>2023</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.39802377999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" t="s">
+        <v>218</v>
+      </c>
+      <c r="C51">
+        <v>2013</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.39548506999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B52" t="s">
+        <v>301</v>
+      </c>
+      <c r="C52">
+        <v>2022</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.39179897000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B53" t="s">
+        <v>330</v>
+      </c>
+      <c r="C53">
+        <v>2010</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.39139032000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54">
+        <v>2018</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.38802432999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55">
+        <v>2020</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.38757205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B56" t="s">
+        <v>271</v>
+      </c>
+      <c r="C56">
+        <v>2013</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.38743453999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57">
+        <v>2021</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.38701963</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58">
+        <v>2019</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.38542736</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59">
+        <v>2022</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.38542363000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60">
+        <v>2023</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.38397565</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61">
+        <v>2022</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.38201501999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62">
+        <v>2017</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.38024372000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63">
+        <v>2021</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.37893850000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B64" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64">
+        <v>2021</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.37858006</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B65" t="s">
+        <v>297</v>
+      </c>
+      <c r="C65">
+        <v>2019</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.37663775999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66">
+        <v>2020</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.37456086</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67">
+        <v>2021</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.37391287000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68">
+        <v>2022</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.37357685000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B69" t="s">
+        <v>287</v>
+      </c>
+      <c r="C69">
+        <v>2012</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.37054925999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70">
+        <v>2017</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.36761206000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B71" t="s">
+        <v>353</v>
+      </c>
+      <c r="C71">
+        <v>2014</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.36707094000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B72" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72">
+        <v>2022</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.3656239</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B73" t="s">
+        <v>244</v>
+      </c>
+      <c r="C73">
+        <v>2023</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.36381876000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B74" t="s">
+        <v>258</v>
+      </c>
+      <c r="C74">
+        <v>2022</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.36252203999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B75" t="s">
+        <v>275</v>
+      </c>
+      <c r="C75">
+        <v>2021</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.36157719999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B76" t="s">
+        <v>351</v>
+      </c>
+      <c r="C76">
+        <v>2022</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.36093006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B77" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77">
+        <v>2020</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.36068243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78">
+        <v>2023</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.35884795000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79">
+        <v>2021</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.35743752000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B80" t="s">
+        <v>281</v>
+      </c>
+      <c r="C80">
+        <v>2018</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.35690176000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B81" t="s">
+        <v>197</v>
+      </c>
+      <c r="C81">
+        <v>2021</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.35653594</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82">
+        <v>2021</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.35652608000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B83" t="s">
+        <v>201</v>
+      </c>
+      <c r="C83">
+        <v>2019</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.35482943</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84">
+        <v>2022</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.35281137000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85">
+        <v>2021</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.35275363999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86">
+        <v>2016</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.35265439999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87">
+        <v>2023</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.35203487</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B88" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88">
+        <v>2017</v>
+      </c>
+      <c r="D88" s="2">
+        <v>0.35128385000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B89" t="s">
+        <v>236</v>
+      </c>
+      <c r="C89">
+        <v>2018</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.35127744</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" t="s">
+        <v>147</v>
+      </c>
+      <c r="C90">
+        <v>2024</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0.34894395</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C91">
+        <v>2023</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.34756895999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B92" t="s">
+        <v>199</v>
+      </c>
+      <c r="C92">
+        <v>2022</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0.34587276</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B93" t="s">
+        <v>345</v>
+      </c>
+      <c r="C93">
+        <v>2023</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.34538773</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94" t="s">
+        <v>30</v>
+      </c>
+      <c r="C94">
+        <v>2021</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0.34395808</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B95" t="s">
+        <v>14</v>
+      </c>
+      <c r="C95">
+        <v>2018</v>
+      </c>
+      <c r="D95" s="2">
+        <v>0.34332526000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B96" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96">
+        <v>2021</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.34296975000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B97" t="s">
+        <v>299</v>
+      </c>
+      <c r="C97">
+        <v>2014</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.34242942999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B98" t="s">
+        <v>187</v>
+      </c>
+      <c r="C98">
+        <v>2022</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.34093987999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99">
+        <v>2016</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.34068036000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B100" t="s">
+        <v>312</v>
+      </c>
+      <c r="C100">
+        <v>2015</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.33995535999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B101" t="s">
+        <v>306</v>
+      </c>
+      <c r="C101">
+        <v>2021</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.33824313</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" t="s">
+        <v>324</v>
+      </c>
+      <c r="C102">
+        <v>2021</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0.33716425</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B103" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103">
+        <v>2022</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.33675845999999998</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B104" t="s">
+        <v>163</v>
+      </c>
+      <c r="C104">
+        <v>2010</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0.3365573</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B105" t="s">
+        <v>157</v>
+      </c>
+      <c r="C105">
+        <v>2022</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.33651528000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B106" t="s">
+        <v>295</v>
+      </c>
+      <c r="C106">
+        <v>2022</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0.33579419999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B107" t="s">
+        <v>238</v>
+      </c>
+      <c r="C107">
+        <v>2019</v>
+      </c>
+      <c r="D107" s="2">
+        <v>0.33505829999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B108" t="s">
+        <v>316</v>
+      </c>
+      <c r="C108">
+        <v>2023</v>
+      </c>
+      <c r="D108" s="2">
+        <v>0.33494889999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B109" t="s">
+        <v>132</v>
+      </c>
+      <c r="C109">
+        <v>2021</v>
+      </c>
+      <c r="D109" s="2">
+        <v>0.33435068000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B110" t="s">
+        <v>124</v>
+      </c>
+      <c r="C110">
+        <v>2022</v>
+      </c>
+      <c r="D110" s="2">
+        <v>0.33373599999999998</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B111" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111">
+        <v>2022</v>
+      </c>
+      <c r="D111" s="2">
+        <v>0.33373155999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B112" t="s">
+        <v>37</v>
+      </c>
+      <c r="C112">
+        <v>2011</v>
+      </c>
+      <c r="D112" s="2">
+        <v>0.33030185000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B113" t="s">
+        <v>291</v>
+      </c>
+      <c r="C113">
+        <v>2021</v>
+      </c>
+      <c r="D113" s="2">
+        <v>0.32906574</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B114" t="s">
+        <v>234</v>
+      </c>
+      <c r="C114">
+        <v>2021</v>
+      </c>
+      <c r="D114" s="2">
+        <v>0.32862564999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B115" t="s">
+        <v>277</v>
+      </c>
+      <c r="C115">
+        <v>2022</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0.32802890000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" t="s">
+        <v>120</v>
+      </c>
+      <c r="C116">
+        <v>2020</v>
+      </c>
+      <c r="D116" s="2">
+        <v>0.32433450000000003</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B117" t="s">
+        <v>338</v>
+      </c>
+      <c r="C117">
+        <v>2021</v>
+      </c>
+      <c r="D117" s="2">
+        <v>0.32414632999999998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" t="s">
+        <v>226</v>
+      </c>
+      <c r="C118">
+        <v>2012</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0.32361580000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B119" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119">
+        <v>2020</v>
+      </c>
+      <c r="D119" s="2">
+        <v>0.32339275000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B120" t="s">
+        <v>347</v>
+      </c>
+      <c r="C120">
+        <v>2019</v>
+      </c>
+      <c r="D120" s="2">
+        <v>0.32317575999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B121" t="s">
+        <v>262</v>
+      </c>
+      <c r="C121">
+        <v>2022</v>
+      </c>
+      <c r="D121" s="2">
+        <v>0.32303035000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B122" t="s">
+        <v>101</v>
+      </c>
+      <c r="C122">
+        <v>2022</v>
+      </c>
+      <c r="D122" s="2">
+        <v>0.32252404000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B123" t="s">
+        <v>279</v>
+      </c>
+      <c r="C123">
+        <v>2018</v>
+      </c>
+      <c r="D123" s="2">
+        <v>0.32125320000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B124" t="s">
+        <v>203</v>
+      </c>
+      <c r="C124">
+        <v>2019</v>
+      </c>
+      <c r="D124" s="2">
+        <v>0.31996748000000003</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B125" t="s">
+        <v>304</v>
+      </c>
+      <c r="C125">
+        <v>2022</v>
+      </c>
+      <c r="D125" s="2">
+        <v>0.31608360000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B126" t="s">
+        <v>310</v>
+      </c>
+      <c r="C126">
+        <v>2021</v>
+      </c>
+      <c r="D126" s="2">
+        <v>0.31566375000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B127" t="s">
+        <v>78</v>
+      </c>
+      <c r="C127">
+        <v>2022</v>
+      </c>
+      <c r="D127" s="2">
+        <v>0.31534076</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B128" t="s">
+        <v>214</v>
+      </c>
+      <c r="C128">
+        <v>2022</v>
+      </c>
+      <c r="D128" s="2">
+        <v>0.31416475999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B129" t="s">
+        <v>112</v>
+      </c>
+      <c r="C129">
+        <v>2022</v>
+      </c>
+      <c r="D129" s="2">
+        <v>0.31236910000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B130" t="s">
+        <v>105</v>
+      </c>
+      <c r="C130">
+        <v>2021</v>
+      </c>
+      <c r="D130" s="2">
+        <v>0.31141794</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B131" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131">
+        <v>2022</v>
+      </c>
+      <c r="D131" s="2">
+        <v>0.30892930000000002</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B132" t="s">
+        <v>108</v>
+      </c>
+      <c r="C132">
+        <v>2019</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0.30706867999999998</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B133" t="s">
+        <v>222</v>
+      </c>
+      <c r="C133">
+        <v>2017</v>
+      </c>
+      <c r="D133" s="2">
+        <v>0.30696869999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C134">
+        <v>2021</v>
+      </c>
+      <c r="D134" s="2">
+        <v>0.30404037</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B135" t="s">
+        <v>141</v>
+      </c>
+      <c r="C135">
+        <v>2022</v>
+      </c>
+      <c r="D135" s="2">
+        <v>0.30222823999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B136" t="s">
+        <v>228</v>
+      </c>
+      <c r="C136">
+        <v>2022</v>
+      </c>
+      <c r="D136" s="2">
+        <v>0.30020264000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B137" t="s">
+        <v>76</v>
+      </c>
+      <c r="C137">
+        <v>2022</v>
+      </c>
+      <c r="D137" s="2">
+        <v>0.30017322000000002</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B138" t="s">
+        <v>153</v>
+      </c>
+      <c r="C138">
+        <v>2022</v>
+      </c>
+      <c r="D138" s="2">
+        <v>0.29912030000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B139" t="s">
+        <v>51</v>
+      </c>
+      <c r="C139">
+        <v>2020</v>
+      </c>
+      <c r="D139" s="2">
+        <v>0.29851684000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B140" t="s">
+        <v>151</v>
+      </c>
+      <c r="C140">
+        <v>2023</v>
+      </c>
+      <c r="D140" s="2">
+        <v>0.29774040000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B141" t="s">
+        <v>130</v>
+      </c>
+      <c r="C141">
+        <v>2018</v>
+      </c>
+      <c r="D141" s="2">
+        <v>0.29591953999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B142" t="s">
+        <v>242</v>
+      </c>
+      <c r="C142">
+        <v>2018</v>
+      </c>
+      <c r="D142" s="2">
+        <v>0.29589265999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>2020</v>
+      </c>
+      <c r="D143" s="2">
+        <v>0.29419630000000002</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B144" t="s">
+        <v>195</v>
+      </c>
+      <c r="C144">
+        <v>2019</v>
+      </c>
+      <c r="D144" s="2">
+        <v>0.29285090000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B145" t="s">
+        <v>84</v>
+      </c>
+      <c r="C145">
+        <v>2022</v>
+      </c>
+      <c r="D145" s="2">
+        <v>0.29259402000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B146" t="s">
+        <v>165</v>
+      </c>
+      <c r="C146">
+        <v>2021</v>
+      </c>
+      <c r="D146" s="2">
+        <v>0.29191532999999997</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B147" t="s">
+        <v>256</v>
+      </c>
+      <c r="C147">
+        <v>2022</v>
+      </c>
+      <c r="D147" s="2">
+        <v>0.28858184999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B148" t="s">
+        <v>90</v>
+      </c>
+      <c r="C148">
+        <v>2014</v>
+      </c>
+      <c r="D148" s="2">
+        <v>0.28652927</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B149" t="s">
+        <v>95</v>
+      </c>
+      <c r="C149">
+        <v>2021</v>
+      </c>
+      <c r="D149" s="2">
+        <v>0.28482037999999998</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B150" t="s">
+        <v>32</v>
+      </c>
+      <c r="C150">
+        <v>2022</v>
+      </c>
+      <c r="D150" s="2">
+        <v>0.2845992</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B151" t="s">
+        <v>110</v>
+      </c>
+      <c r="C151">
+        <v>2022</v>
+      </c>
+      <c r="D151" s="2">
+        <v>0.27925923000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B152" t="s">
+        <v>169</v>
+      </c>
+      <c r="C152">
+        <v>2019</v>
+      </c>
+      <c r="D152" s="2">
+        <v>0.27832701999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B153" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153">
+        <v>2011</v>
+      </c>
+      <c r="D153" s="2">
+        <v>0.27615731999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B154" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154">
+        <v>2023</v>
+      </c>
+      <c r="D154" s="2">
+        <v>0.27154650000000002</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B155" t="s">
+        <v>320</v>
+      </c>
+      <c r="C155">
+        <v>2021</v>
+      </c>
+      <c r="D155" s="2">
+        <v>0.27095764999999999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B156" t="s">
+        <v>240</v>
+      </c>
+      <c r="C156">
+        <v>2022</v>
+      </c>
+      <c r="D156" s="2">
+        <v>0.26946252999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B157" t="s">
+        <v>308</v>
+      </c>
+      <c r="C157">
+        <v>2022</v>
+      </c>
+      <c r="D157" s="2">
+        <v>0.26628074000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B158" t="s">
+        <v>143</v>
+      </c>
+      <c r="C158">
+        <v>2018</v>
+      </c>
+      <c r="D158" s="2">
+        <v>0.2656501</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B159" t="s">
+        <v>336</v>
+      </c>
+      <c r="C159">
+        <v>2018</v>
+      </c>
+      <c r="D159" s="2">
+        <v>0.26399003999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B160" t="s">
+        <v>26</v>
+      </c>
+      <c r="C160">
+        <v>2022</v>
+      </c>
+      <c r="D160" s="2">
+        <v>0.26375556</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B161" t="s">
+        <v>173</v>
+      </c>
+      <c r="C161">
+        <v>2022</v>
+      </c>
+      <c r="D161" s="2">
+        <v>0.26352527999999997</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B162" t="s">
+        <v>80</v>
+      </c>
+      <c r="C162">
+        <v>2022</v>
+      </c>
+      <c r="D162" s="2">
+        <v>0.25870389999999999</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B163" t="s">
+        <v>212</v>
+      </c>
+      <c r="C163">
+        <v>2022</v>
+      </c>
+      <c r="D163" s="2">
+        <v>0.25864446000000002</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B164" t="s">
+        <v>230</v>
+      </c>
+      <c r="C164">
+        <v>2021</v>
+      </c>
+      <c r="D164" s="2">
+        <v>0.25743870000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B165" t="s">
+        <v>334</v>
+      </c>
+      <c r="C165">
+        <v>2020</v>
+      </c>
+      <c r="D165" s="2">
+        <v>0.25627362999999997</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B166" t="s">
+        <v>145</v>
+      </c>
+      <c r="C166">
+        <v>2022</v>
+      </c>
+      <c r="D166" s="2">
+        <v>0.25514996000000001</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B167" t="s">
+        <v>24</v>
+      </c>
+      <c r="C167">
+        <v>2020</v>
+      </c>
+      <c r="D167" s="2">
+        <v>0.24383356</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B168" t="s">
+        <v>285</v>
+      </c>
+      <c r="C168">
+        <v>2022</v>
+      </c>
+      <c r="D168" s="2">
+        <v>0.24305065000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B169" t="s">
+        <v>283</v>
+      </c>
+      <c r="C169">
+        <v>2022</v>
+      </c>
+      <c r="D169" s="2">
+        <v>0.24078926</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>